<commit_message>
Enhance Next.js configuration to remove console logs in production and add pdf-lib dependency for PDF processing. Update PDFProcessor component to validate single-page PDF uploads and adjust Excel population logic for better readability.
</commit_message>
<xml_diff>
--- a/automation/template.xlsx
+++ b/automation/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Files/quote-flow-freight-glide/automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Files/pdf-extract/automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4332F78C-755D-744D-9407-B8C6EA94C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDD06F0-D1FE-6E40-B238-7D0DAE8C7029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9AAD7B7D-03AD-426F-BDAB-20A3D4EAF950}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{9AAD7B7D-03AD-426F-BDAB-20A3D4EAF950}"/>
   </bookViews>
   <sheets>
     <sheet name="NSLJ TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -684,35 +684,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1073,7 +1073,7 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1100,68 +1100,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="63.75" customHeight="1">
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="2:15" ht="16.5" customHeight="1">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
     </row>
     <row r="3" spans="2:15" ht="16.5" customHeight="1">
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
     </row>
     <row r="4" spans="2:15" ht="16.5" customHeight="1">
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
     </row>
     <row r="5" spans="2:15">
       <c r="B5" s="1"/>
@@ -1198,22 +1198,22 @@
       <c r="O6" s="52"/>
     </row>
     <row r="7" spans="2:15" ht="34.5" customHeight="1">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" s="1"/>
@@ -1235,88 +1235,88 @@
       <c r="B9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="60" t="s">
+      <c r="K9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="60"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" s="46"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="61" t="s">
+      <c r="K10" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="62"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="55"/>
     </row>
     <row r="11" spans="2:15" ht="17.25" customHeight="1">
       <c r="B11" s="47"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="20"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
     </row>
     <row r="12" spans="2:15" ht="16.5" customHeight="1">
       <c r="B12" s="47"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="20"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="62"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="46"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="20"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="60" t="s">
+      <c r="K13" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="62"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" s="1"/>
@@ -1328,12 +1328,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="61" t="s">
+      <c r="K14" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="62"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="55"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="2:15">
@@ -1446,7 +1446,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="9"/>
       <c r="L19" s="10">
-        <f>ROUND((G19*H19*I19)/1000000, 3)</f>
+        <f>ROUND((G19*H19*I19), 3)</f>
         <v>0</v>
       </c>
       <c r="M19" s="8"/>
@@ -1742,6 +1742,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B7:O7"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B4:O4"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="K9:L9"/>
@@ -1754,16 +1764,6 @@
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B7:O7"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B4:O4"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -1773,6 +1773,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f86f3b12-551f-42f7-855b-cf98681be652">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fb3033b4-e847-4e4b-b8a1-936d9de62bbf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B5DE500CDDDBA0449D36630E076BFA98" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a86883071cf411f184bd3f9daee7057e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f86f3b12-551f-42f7-855b-cf98681be652" xmlns:ns3="fb3033b4-e847-4e4b-b8a1-936d9de62bbf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84533ae0880d7bef7f9189d15193b940" ns2:_="" ns3:_="">
     <xsd:import namespace="f86f3b12-551f-42f7-855b-cf98681be652"/>
@@ -1967,27 +1987,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5875F3FE-D9D4-41A3-9CC1-53CB2A7FE56D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f86f3b12-551f-42f7-855b-cf98681be652"/>
+    <ds:schemaRef ds:uri="fb3033b4-e847-4e4b-b8a1-936d9de62bbf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f86f3b12-551f-42f7-855b-cf98681be652">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fb3033b4-e847-4e4b-b8a1-936d9de62bbf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC75C3B-A275-49BD-AAF3-948539194E1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21E1BB96-47CC-43A5-8286-0F3E5E29F3A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2004,23 +2023,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC75C3B-A275-49BD-AAF3-948539194E1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5875F3FE-D9D4-41A3-9CC1-53CB2A7FE56D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f86f3b12-551f-42f7-855b-cf98681be652"/>
-    <ds:schemaRef ds:uri="fb3033b4-e847-4e4b-b8a1-936d9de62bbf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>